<commit_message>
Upload WB040 DNA Purification
</commit_message>
<xml_diff>
--- a/labnote/001_oligo_assembly_test_GFP-mCherry/resources/Plate_Layout_Concentration.xlsx
+++ b/labnote/001_oligo_assembly_test_GFP-mCherry/resources/Plate_Layout_Concentration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\workspace\labnote\labnote\oligo_assembly_SOP\labnote\001_oligo_assembly_test_GFP-mCherry\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC17BB3-0E7D-401E-8ADD-D882039F5BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3729733C-B228-4D09-9B11-2B4547C565A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-30" windowWidth="16440" windowHeight="28320" xr2:uid="{2480BB0B-75BD-42E7-8E2F-63248CEE8E3E}"/>
   </bookViews>
@@ -398,6 +398,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +440,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -446,6 +449,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B415528-C3DF-4BF4-9A29-40D2E0235B50}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.600000000000001" x14ac:dyDescent="0.55000000000000004"/>
@@ -793,7 +799,7 @@
     <col min="2" max="2" width="19.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,7 +807,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -812,7 +818,7 @@
         <v>90.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -823,7 +829,7 @@
         <v>78.2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -834,7 +840,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -845,7 +851,7 @@
         <v>69.8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -856,7 +862,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -867,7 +873,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -878,7 +884,7 @@
         <v>50.6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -889,7 +895,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -900,7 +906,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -911,7 +917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -922,7 +928,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -932,8 +938,12 @@
       <c r="C13">
         <v>32.1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" s="3">
+        <f>AVERAGE(C2:C13)</f>
+        <v>59.183333333333337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -944,7 +954,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -955,7 +965,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1318,7 +1328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -1327,6 +1337,10 @@
       </c>
       <c r="C49">
         <v>11</v>
+      </c>
+      <c r="E49" s="3">
+        <f>AVERAGE(C14:C49)</f>
+        <v>22.863888888888894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>